<commit_message>
coneccion para el memo
</commit_message>
<xml_diff>
--- a/public/test.xlsx
+++ b/public/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\inventarioInformatico\stock\stockBackend\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BD3D6B-C06E-470B-9A3D-00E90218F5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7A2FC1-06BD-4AB4-B3DB-F98A7975F3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>${name}</t>
+    <t>${table:people.name}</t>
   </si>
 </sst>
 </file>

</xml_diff>